<commit_message>
Created Database Table Columns
</commit_message>
<xml_diff>
--- a/src/main/resource/Employee.xlsx
+++ b/src/main/resource/Employee.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenit\eclipse-workspace\Importer\src\main\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenit\Desktop\Git Repo\ExcelImporter\src\main\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E0EF6FB-EF18-4D61-9C37-E32BC26D86E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB83688B-2718-4C80-9591-1B5A7E4EDC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53BD86E4-793E-4C5F-93E8-543548F9CBCC}"/>
   </bookViews>
@@ -27,16 +27,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
     <t>Kenit</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -401,13 +401,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -415,7 +415,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>999999999</v>
@@ -426,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>999999999</v>
@@ -437,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>999999999</v>
@@ -448,7 +448,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>999999999</v>
@@ -459,7 +459,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>999999999</v>
@@ -470,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>999999999</v>

</xml_diff>